<commit_message>
small edits to plot template & example plot
</commit_message>
<xml_diff>
--- a/plot_template.xlsx
+++ b/plot_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28360" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="28360" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -4848,7 +4848,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4865,6 +4865,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4938,7 +4956,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4962,6 +4980,15 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4985,10 +5012,19 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="15"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -4996,16 +5032,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5059,6 +5085,156 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -5085,7 +5261,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Turnstile Traffic at 42 ST-BRYANT PK, 2/2 - 9/2 2013</c:v>
+              <c:v>Turnstile Traffic at 42 ST-BRYANT PK, 2/2 - 2/9 2013</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -5113,127 +5289,127 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>2/2 3:00 - 2/2 7:00</c:v>
+                  <c:v>Sat 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/2 7:00 - 2/2 11:00</c:v>
+                  <c:v>Sat 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/2 11:00 - 2/2 15:00</c:v>
+                  <c:v>Sat 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/2 15:00 - 2/2 19:00</c:v>
+                  <c:v>Sat 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/2 19:00 - 2/2 23:00</c:v>
+                  <c:v>Sat 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/2 23:00 - 3/2 3:00</c:v>
+                  <c:v>Sat 11 PM - Sun 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3/2 3:00 - 3/2 7:00</c:v>
+                  <c:v>Sun 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3/2 7:00 - 3/2 11:00</c:v>
+                  <c:v>Sun 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3/2 11:00 - 3/2 15:00</c:v>
+                  <c:v>Sun 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3/2 15:00 - 3/2 19:00</c:v>
+                  <c:v>Sun 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3/2 19:00 - 3/2 23:00</c:v>
+                  <c:v>Sun 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3/2 23:00 - 4/2 3:00</c:v>
+                  <c:v>Sun 11 PM - Mon 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4/2 3:00 - 4/2 7:00</c:v>
+                  <c:v>Mon 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4/2 7:00 - 4/2 11:00</c:v>
+                  <c:v>Mon 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4/2 11:00 - 4/2 15:00</c:v>
+                  <c:v>Mon 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4/2 15:00 - 4/2 19:00</c:v>
+                  <c:v>Mon 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4/2 19:00 - 4/2 23:00</c:v>
+                  <c:v>Mon 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4/2 23:00 - 5/2 3:00</c:v>
+                  <c:v>Mon 11 PM - Tue 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5/2 3:00 - 5/2 7:00</c:v>
+                  <c:v>Tue 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5/2 7:00 - 5/2 11:00</c:v>
+                  <c:v>Tue 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5/2 11:00 - 5/2 15:00</c:v>
+                  <c:v>Tue 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5/2 15:00 - 5/2 19:00</c:v>
+                  <c:v>Tue 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5/2 19:00 - 5/2 23:00</c:v>
+                  <c:v>Tue 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5/2 23:00 - 6/2 3:00</c:v>
+                  <c:v>Tue 11 PM - Wed 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6/2 3:00 - 6/2 7:00</c:v>
+                  <c:v>Wed 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6/2 7:00 - 6/2 11:00</c:v>
+                  <c:v>Wed 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6/2 11:00 - 6/2 15:00</c:v>
+                  <c:v>Wed 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6/2 15:00 - 6/2 19:00</c:v>
+                  <c:v>Wed 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6/2 19:00 - 6/2 23:00</c:v>
+                  <c:v>Wed 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6/2 23:00 - 7/2 3:00</c:v>
+                  <c:v>Wed 11 PM - Thu 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7/2 3:00 - 7/2 7:00</c:v>
+                  <c:v>Thu 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7/2 7:00 - 7/2 11:00</c:v>
+                  <c:v>Thu 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7/2 11:00 - 7/2 15:00</c:v>
+                  <c:v>Thu 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7/2 15:00 - 7/2 19:00</c:v>
+                  <c:v>Thu 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7/2 19:00 - 7/2 23:00</c:v>
+                  <c:v>Thu 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7/2 23:00 - 8/2 3:00</c:v>
+                  <c:v>Thu 11 PM - Fri 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8/2 3:00 - 8/2 7:00</c:v>
+                  <c:v>Fri 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8/2 7:00 - 8/2 11:00</c:v>
+                  <c:v>Fri 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8/2 11:00 - 8/2 15:00</c:v>
+                  <c:v>Fri 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8/2 15:00 - 8/2 19:00</c:v>
+                  <c:v>Fri 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8/2 19:00 - 8/2 23:00</c:v>
+                  <c:v>Fri 7 PM - 11 PM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5384,127 +5560,127 @@
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>2/2 3:00 - 2/2 7:00</c:v>
+                  <c:v>Sat 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/2 7:00 - 2/2 11:00</c:v>
+                  <c:v>Sat 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/2 11:00 - 2/2 15:00</c:v>
+                  <c:v>Sat 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/2 15:00 - 2/2 19:00</c:v>
+                  <c:v>Sat 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2/2 19:00 - 2/2 23:00</c:v>
+                  <c:v>Sat 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2/2 23:00 - 3/2 3:00</c:v>
+                  <c:v>Sat 11 PM - Sun 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3/2 3:00 - 3/2 7:00</c:v>
+                  <c:v>Sun 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3/2 7:00 - 3/2 11:00</c:v>
+                  <c:v>Sun 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3/2 11:00 - 3/2 15:00</c:v>
+                  <c:v>Sun 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3/2 15:00 - 3/2 19:00</c:v>
+                  <c:v>Sun 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3/2 19:00 - 3/2 23:00</c:v>
+                  <c:v>Sun 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3/2 23:00 - 4/2 3:00</c:v>
+                  <c:v>Sun 11 PM - Mon 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4/2 3:00 - 4/2 7:00</c:v>
+                  <c:v>Mon 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4/2 7:00 - 4/2 11:00</c:v>
+                  <c:v>Mon 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4/2 11:00 - 4/2 15:00</c:v>
+                  <c:v>Mon 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4/2 15:00 - 4/2 19:00</c:v>
+                  <c:v>Mon 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4/2 19:00 - 4/2 23:00</c:v>
+                  <c:v>Mon 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4/2 23:00 - 5/2 3:00</c:v>
+                  <c:v>Mon 11 PM - Tue 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5/2 3:00 - 5/2 7:00</c:v>
+                  <c:v>Tue 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5/2 7:00 - 5/2 11:00</c:v>
+                  <c:v>Tue 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5/2 11:00 - 5/2 15:00</c:v>
+                  <c:v>Tue 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5/2 15:00 - 5/2 19:00</c:v>
+                  <c:v>Tue 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5/2 19:00 - 5/2 23:00</c:v>
+                  <c:v>Tue 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5/2 23:00 - 6/2 3:00</c:v>
+                  <c:v>Tue 11 PM - Wed 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6/2 3:00 - 6/2 7:00</c:v>
+                  <c:v>Wed 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6/2 7:00 - 6/2 11:00</c:v>
+                  <c:v>Wed 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6/2 11:00 - 6/2 15:00</c:v>
+                  <c:v>Wed 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6/2 15:00 - 6/2 19:00</c:v>
+                  <c:v>Wed 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6/2 19:00 - 6/2 23:00</c:v>
+                  <c:v>Wed 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6/2 23:00 - 7/2 3:00</c:v>
+                  <c:v>Wed 11 PM - Thu 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7/2 3:00 - 7/2 7:00</c:v>
+                  <c:v>Thu 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7/2 7:00 - 7/2 11:00</c:v>
+                  <c:v>Thu 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7/2 11:00 - 7/2 15:00</c:v>
+                  <c:v>Thu 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7/2 15:00 - 7/2 19:00</c:v>
+                  <c:v>Thu 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7/2 19:00 - 7/2 23:00</c:v>
+                  <c:v>Thu 7 PM - 11 PM</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7/2 23:00 - 8/2 3:00</c:v>
+                  <c:v>Thu 11 PM - Fri 3 AM</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8/2 3:00 - 8/2 7:00</c:v>
+                  <c:v>Fri 3 AM - 7 AM</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8/2 7:00 - 8/2 11:00</c:v>
+                  <c:v>Fri 7 AM - 11 AM</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8/2 11:00 - 8/2 15:00</c:v>
+                  <c:v>Fri 11 AM - 3 PM</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8/2 15:00 - 8/2 19:00</c:v>
+                  <c:v>Fri 3 PM - 7 PM</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8/2 19:00 - 8/2 23:00</c:v>
+                  <c:v>Fri 7 PM - 11 PM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5651,11 +5827,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="112464088"/>
-        <c:axId val="112447768"/>
+        <c:axId val="554717080"/>
+        <c:axId val="554714088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="112464088"/>
+        <c:axId val="554717080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5664,7 +5840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112447768"/>
+        <c:crossAx val="554714088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5672,7 +5848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112447768"/>
+        <c:axId val="554714088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -5684,7 +5860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112464088"/>
+        <c:crossAx val="554717080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5725,7 +5901,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8569919" cy="5823415"/>
+    <xdr:ext cx="8581402" cy="5839626"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -6074,7 +6250,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6177,15 +6353,15 @@
         <v>114050333</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>TEXT(A4,"D/M h:mm")&amp;" - "&amp;TEXT(A5,"D/M h:mm")</f>
-        <v>2/2 3:00 - 2/2 7:00</v>
+        <f>TEXT(A4,"ddd h AM/PM")&amp;" - "&amp;TEXT(A5,"h AM/PM")</f>
+        <v>Sat 3 AM - 7 AM</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E39" si="0">B5-B4</f>
+        <f t="shared" ref="E4" si="0">B5-B4</f>
         <v>28570342</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F39" si="1">C5-C4</f>
+        <f t="shared" ref="F4" si="1">C5-C4</f>
         <v>13861361</v>
       </c>
       <c r="I4" s="25"/>
@@ -6207,15 +6383,15 @@
         <v>127911694</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f t="shared" ref="D5:D44" si="2">TEXT(A5,"D/M h:mm")&amp;" - "&amp;TEXT(A6,"D/M h:mm")</f>
-        <v>2/2 7:00 - 2/2 11:00</v>
+        <f t="shared" ref="D5:D44" si="2">TEXT(A5,"ddd h AM/PM")&amp;" - "&amp;TEXT(A6,"h AM/PM")</f>
+        <v>Sat 7 AM - 11 AM</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E5" si="3">B6-B5</f>
         <v>788</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F4:F5" si="4">C6-C5</f>
         <v>3068</v>
       </c>
       <c r="I5" s="20"/>
@@ -6239,7 +6415,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2/2 11:00 - 2/2 15:00</v>
+        <v>Sat 11 AM - 3 PM</v>
       </c>
       <c r="E6" s="3">
         <f>B7-B6</f>
@@ -6250,8 +6426,8 @@
         <v>4150</v>
       </c>
       <c r="O6" t="str">
-        <f>"Turnstile Traffic at "&amp;O5&amp;", "&amp;TEXT(A4,"D/M")&amp;" - "&amp;TEXT(A5+7,"D/M YYYY")</f>
-        <v>Turnstile Traffic at 42 ST-BRYANT PK, 2/2 - 9/2 2013</v>
+        <f>"Turnstile Traffic at "&amp;O5&amp;", "&amp;TEXT(A4,"M/D")&amp;" - "&amp;TEXT(A5+7,"M/D YYYY")</f>
+        <v>Turnstile Traffic at 42 ST-BRYANT PK, 2/2 - 2/9 2013</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -6266,14 +6442,14 @@
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2/2 15:00 - 2/2 19:00</v>
+        <v>Sat 3 PM - 7 PM</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" ref="E7:E39" si="3">B8-B7</f>
+        <f t="shared" ref="E7:E39" si="5">B8-B7</f>
         <v>5135</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F7:F39" si="4">C8-C7</f>
+        <f t="shared" ref="F7:F39" si="6">C8-C7</f>
         <v>4326</v>
       </c>
     </row>
@@ -6289,14 +6465,14 @@
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>2/2 19:00 - 2/2 23:00</v>
+        <v>Sat 7 PM - 11 PM</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3102</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2168</v>
       </c>
     </row>
@@ -6311,15 +6487,15 @@
         <v>127925406</v>
       </c>
       <c r="D9" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>2/2 23:00 - 3/2 3:00</v>
+        <f>TEXT(A9,"ddd h AM/PM")&amp;" - "&amp;TEXT(A10,"ddd h AM/PM")</f>
+        <v>Sat 11 PM - Sun 3 AM</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1757</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>770</v>
       </c>
     </row>
@@ -6335,14 +6511,14 @@
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>3/2 3:00 - 3/2 7:00</v>
+        <v>Sun 3 AM - 7 AM</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>254</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>385</v>
       </c>
     </row>
@@ -6358,14 +6534,14 @@
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>3/2 7:00 - 3/2 11:00</v>
+        <v>Sun 7 AM - 11 AM</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>535</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1839</v>
       </c>
     </row>
@@ -6381,14 +6557,14 @@
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>3/2 11:00 - 3/2 15:00</v>
+        <v>Sun 11 AM - 3 PM</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1554</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3129</v>
       </c>
     </row>
@@ -6404,14 +6580,14 @@
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>3/2 15:00 - 3/2 19:00</v>
+        <v>Sun 3 PM - 7 PM</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3439</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2944</v>
       </c>
     </row>
@@ -6427,14 +6603,14 @@
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>3/2 19:00 - 3/2 23:00</v>
+        <v>Sun 7 PM - 11 PM</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2020</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>804</v>
       </c>
     </row>
@@ -6449,15 +6625,15 @@
         <v>127935277</v>
       </c>
       <c r="D15" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>3/2 23:00 - 4/2 3:00</v>
+        <f>TEXT(A15,"ddd h AM/PM")&amp;" - "&amp;TEXT(A16,"ddd h AM/PM")</f>
+        <v>Sun 11 PM - Mon 3 AM</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>843</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>453</v>
       </c>
     </row>
@@ -6473,14 +6649,14 @@
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>4/2 3:00 - 4/2 7:00</v>
+        <v>Mon 3 AM - 7 AM</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1565</v>
       </c>
     </row>
@@ -6496,14 +6672,14 @@
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>4/2 7:00 - 4/2 11:00</v>
+        <v>Mon 7 AM - 11 AM</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2062</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18905</v>
       </c>
     </row>
@@ -6519,14 +6695,14 @@
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>4/2 11:00 - 4/2 15:00</v>
+        <v>Mon 11 AM - 3 PM</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4820</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5743</v>
       </c>
     </row>
@@ -6542,14 +6718,14 @@
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>4/2 15:00 - 4/2 19:00</v>
+        <v>Mon 3 PM - 7 PM</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20757</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6087</v>
       </c>
     </row>
@@ -6565,14 +6741,14 @@
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>4/2 19:00 - 4/2 23:00</v>
+        <v>Mon 7 PM - 11 PM</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8574</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1444</v>
       </c>
     </row>
@@ -6587,15 +6763,15 @@
         <v>127969474</v>
       </c>
       <c r="D21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>4/2 23:00 - 5/2 3:00</v>
+        <f>TEXT(A21,"ddd h AM/PM")&amp;" - "&amp;TEXT(A22,"ddd h AM/PM")</f>
+        <v>Mon 11 PM - Tue 3 AM</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1227</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>320</v>
       </c>
     </row>
@@ -6611,14 +6787,14 @@
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>5/2 3:00 - 5/2 7:00</v>
+        <v>Tue 3 AM - 7 AM</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>320</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1684</v>
       </c>
     </row>
@@ -6634,14 +6810,14 @@
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>5/2 7:00 - 5/2 11:00</v>
+        <v>Tue 7 AM - 11 AM</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2238</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21550</v>
       </c>
     </row>
@@ -6657,14 +6833,14 @@
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>5/2 11:00 - 5/2 15:00</v>
+        <v>Tue 11 AM - 3 PM</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5183</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6204</v>
       </c>
     </row>
@@ -6680,14 +6856,14 @@
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>5/2 15:00 - 5/2 19:00</v>
+        <v>Tue 3 PM - 7 PM</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21381</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6384</v>
       </c>
     </row>
@@ -6703,14 +6879,14 @@
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>5/2 19:00 - 5/2 23:00</v>
+        <v>Tue 7 PM - 11 PM</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9600</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1660</v>
       </c>
     </row>
@@ -6725,15 +6901,15 @@
         <v>128007276</v>
       </c>
       <c r="D27" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>5/2 23:00 - 6/2 3:00</v>
+        <f>TEXT(A27,"ddd h AM/PM")&amp;" - "&amp;TEXT(A28,"ddd h AM/PM")</f>
+        <v>Tue 11 PM - Wed 3 AM</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1339</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>331</v>
       </c>
     </row>
@@ -6749,14 +6925,14 @@
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>6/2 3:00 - 6/2 7:00</v>
+        <v>Wed 3 AM - 7 AM</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>348</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1645</v>
       </c>
     </row>
@@ -6772,14 +6948,14 @@
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>6/2 7:00 - 6/2 11:00</v>
+        <v>Wed 7 AM - 11 AM</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2145</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21420</v>
       </c>
     </row>
@@ -6795,14 +6971,14 @@
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>6/2 11:00 - 6/2 15:00</v>
+        <v>Wed 11 AM - 3 PM</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5314</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6427</v>
       </c>
     </row>
@@ -6818,14 +6994,14 @@
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>6/2 15:00 - 6/2 19:00</v>
+        <v>Wed 3 PM - 7 PM</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21350</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6629</v>
       </c>
     </row>
@@ -6841,14 +7017,14 @@
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>6/2 19:00 - 6/2 23:00</v>
+        <v>Wed 7 PM - 11 PM</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9984</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1755</v>
       </c>
     </row>
@@ -6863,15 +7039,15 @@
         <v>128045483</v>
       </c>
       <c r="D33" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>6/2 23:00 - 7/2 3:00</v>
+        <f>TEXT(A33,"ddd h AM/PM")&amp;" - "&amp;TEXT(A34,"ddd h AM/PM")</f>
+        <v>Wed 11 PM - Thu 3 AM</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1415</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>362</v>
       </c>
     </row>
@@ -6887,14 +7063,14 @@
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>7/2 3:00 - 7/2 7:00</v>
+        <v>Thu 3 AM - 7 AM</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>336</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
@@ -6910,14 +7086,14 @@
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>7/2 7:00 - 7/2 11:00</v>
+        <v>Thu 7 AM - 11 AM</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2341</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21425</v>
       </c>
     </row>
@@ -6933,14 +7109,14 @@
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>7/2 11:00 - 7/2 15:00</v>
+        <v>Thu 11 AM - 3 PM</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5446188</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-4112526</v>
       </c>
     </row>
@@ -6956,14 +7132,14 @@
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>7/2 15:00 - 7/2 19:00</v>
+        <v>Thu 3 PM - 7 PM</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2360565</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-110398</v>
       </c>
     </row>
@@ -6979,14 +7155,14 @@
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>7/2 19:00 - 7/2 23:00</v>
+        <v>Thu 7 PM - 11 PM</v>
       </c>
       <c r="E38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3122761</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4238798</v>
       </c>
     </row>
@@ -7001,15 +7177,15 @@
         <v>128084834</v>
       </c>
       <c r="D39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>7/2 23:00 - 8/2 3:00</v>
+        <f>TEXT(A39,"ddd h AM/PM")&amp;" - "&amp;TEXT(A40,"ddd h AM/PM")</f>
+        <v>Thu 11 PM - Fri 3 AM</v>
       </c>
       <c r="E39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1568</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>393</v>
       </c>
     </row>
@@ -7025,14 +7201,14 @@
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>8/2 3:00 - 8/2 7:00</v>
+        <v>Fri 3 AM - 7 AM</v>
       </c>
       <c r="E40" s="3">
-        <f>B41-B40</f>
+        <f t="shared" ref="E40:F44" si="7">B41-B40</f>
         <v>369</v>
       </c>
       <c r="F40" s="3">
-        <f>C41-C40</f>
+        <f t="shared" si="7"/>
         <v>1620</v>
       </c>
     </row>
@@ -7048,14 +7224,14 @@
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>8/2 7:00 - 8/2 11:00</v>
+        <v>Fri 7 AM - 11 AM</v>
       </c>
       <c r="E41" s="3">
-        <f>B42-B41</f>
+        <f t="shared" si="7"/>
         <v>2099</v>
       </c>
       <c r="F41" s="3">
-        <f>C42-C41</f>
+        <f t="shared" si="7"/>
         <v>18433</v>
       </c>
     </row>
@@ -7071,14 +7247,14 @@
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>8/2 11:00 - 8/2 15:00</v>
+        <v>Fri 11 AM - 3 PM</v>
       </c>
       <c r="E42" s="3">
-        <f>B43-B42</f>
+        <f t="shared" si="7"/>
         <v>8721</v>
       </c>
       <c r="F42" s="3">
-        <f>C43-C42</f>
+        <f t="shared" si="7"/>
         <v>5049</v>
       </c>
     </row>
@@ -7094,14 +7270,14 @@
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>8/2 15:00 - 8/2 19:00</v>
+        <v>Fri 3 PM - 7 PM</v>
       </c>
       <c r="E43" s="3">
-        <f>B44-B43</f>
+        <f t="shared" si="7"/>
         <v>16176</v>
       </c>
       <c r="F43" s="3">
-        <f>C44-C43</f>
+        <f t="shared" si="7"/>
         <v>3664</v>
       </c>
       <c r="H43" s="13"/>
@@ -7122,14 +7298,14 @@
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>8/2 19:00 - 8/2 23:00</v>
+        <v>Fri 7 PM - 11 PM</v>
       </c>
       <c r="E44" s="3">
-        <f>B45-B44</f>
+        <f t="shared" si="7"/>
         <v>3059</v>
       </c>
       <c r="F44" s="3">
-        <f>C45-C44</f>
+        <f t="shared" si="7"/>
         <v>786</v>
       </c>
     </row>
@@ -7185,15 +7361,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:F44">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>30000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:F44">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+  <conditionalFormatting sqref="E40:F44 D4:D44 D4:F39">
+    <cfRule type="containsBlanks" dxfId="6" priority="2">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>